<commit_message>
added api for some features
</commit_message>
<xml_diff>
--- a/src/main/resources/womenBoohooDress.xlsx
+++ b/src/main/resources/womenBoohooDress.xlsx
@@ -12,9 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="93">
-  <si>
-    <t>Category</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="116">
+  <si>
+    <t>Id</t>
   </si>
   <si>
     <t>Image</t>
@@ -32,7 +32,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>WOMEN DRESS</t>
+    <t>women_boohoo_dress_1</t>
   </si>
   <si>
     <t>https://media.boohoo.com/i/boohoo/gzz92062_pink_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
@@ -44,253 +44,322 @@
     <t>MOLLY SMITH HALTER PRINTED RUFFLE MESH MINI DRESS</t>
   </si>
   <si>
+    <t>$30.00</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/molly-smith-halter-printed-ruffle-mesh-mini-dress/GZZ92062.html?color=155</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_2</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz91966_hot%20pink_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>MOLLY SMITH PLUNGE ZEBRA ACETATE SLINKY CUT OUT MINI DRESS</t>
+  </si>
+  <si>
     <t>$74.50</t>
   </si>
   <si>
-    <t>https://ca.boohoo.com/molly-smith-halter-printed-ruffle-mesh-mini-dress/GZZ92062.html?color=155</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz91966_hot%20pink_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>MOLLY SMITH PLUNGE ZEBRA ACETATE SLINKY CUT OUT MINI DRESS</t>
-  </si>
-  <si>
-    <t>$20.00</t>
-  </si>
-  <si>
     <t>https://ca.boohoo.com/molly-smith-plunge-zebra-acetate-slinky-cut-out-mini-dress-/GZZ91966.html?color=535</t>
   </si>
   <si>
+    <t>women_boohoo_dress_3</t>
+  </si>
+  <si>
     <t>https://media.boohoo.com/i/boohoo/gzz91918_hot%20pink_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
   </si>
   <si>
     <t>MOLLY SMITH BANDEAU TRIM CUT OUT MINI DRESS</t>
   </si>
   <si>
-    <t>$30.00</t>
+    <t>$46.50</t>
   </si>
   <si>
     <t>https://ca.boohoo.com/molly-smith-bandeau-trim-cut-out-mini-dress/GZZ91918.html?color=535</t>
   </si>
   <si>
+    <t>women_boohoo_dress_4</t>
+  </si>
+  <si>
     <t>https://media.boohoo.com/i/boohoo/gzz91923_leopard_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
   </si>
   <si>
     <t>MOLLY SMITH LEOPARD CUT OUT MESH MIDAXI DRESS</t>
   </si>
   <si>
-    <t>$32.50</t>
-  </si>
-  <si>
     <t>https://ca.boohoo.com/molly-smith-leopard-cut-out-mesh-midaxi-dress/GZZ91923.html?color=193</t>
   </si>
   <si>
+    <t>women_boohoo_dress_5</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz94131_multi_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>MOLLY SMITH COWL NECK TIE FRONT PRINTED MAXI DRESS</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/molly-smith-cowl-neck-tie-front-printed-maxi-dress/GZZ94131.html?color=144</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_6</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz91938_brown_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>MOLLY SMITH LACE TRIM LEOPARD MESH MINI DRESS</t>
+  </si>
+  <si>
+    <t>$66.00</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/molly-smith-lace-trim-leopard-mesh-mini-dress/GZZ91938.html</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_7</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz92887_brown_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>MOLLY SMITH MIX PRINT RUCHED MINI DRESS</t>
+  </si>
+  <si>
+    <t>$63.00</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/molly-smith-mix-print-ruched-mini-dress/GZZ92887.html</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_8</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz94022_black_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>MOLLY SMITH SQUARE NECK STRAPPY LACE MAXI DRESS</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/molly-smith-square-neck-strappy-lace-maxi-dress/GZZ94022.html?color=105</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_9</t>
+  </si>
+  <si>
     <t>https://media.boohoo.com/i/boohoo/gzz91920_yellow_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
   </si>
   <si>
+    <t>https://ca.boohoo.com/molly-smith-bandeau-trim-cut-out-mini-dress/GZZ91920.html</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_10</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz91984_pink_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>MOLLY SMITH RUCHED SLINKY CUT OUT MAXI DRESS</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/molly-smith-ruched-slinky-cut-out-maxi-dress/GZZ91984.html?color=155</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_11</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz89419_white_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>MOLLY SMITH BANDEAU RUFFLE ASSYMETRIC DEVORE MINI DRESS</t>
+  </si>
+  <si>
+    <t>$53.00</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/molly-smith-bandeau-ruffle-assymetric-devore-mini-dress/GZZ89419.html</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_12</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz92889_brown_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>MOLLY SMITH FLORAL TIE FRONT MAXI DRESS</t>
+  </si>
+  <si>
     <t>$37.00</t>
   </si>
   <si>
-    <t>https://ca.boohoo.com/molly-smith-bandeau-trim-cut-out-mini-dress/GZZ91920.html</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz94131_multi_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>MOLLY SMITH COWL NECK TIE FRONT PRINTED MAXI DRESS</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/molly-smith-cowl-neck-tie-front-printed-maxi-dress/GZZ94131.html?color=144</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz91938_brown_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>MOLLY SMITH LACE TRIM LEOPARD MESH MINI DRESS</t>
+    <t>https://ca.boohoo.com/molly-smith-floral-tie-front-maxi-dress/GZZ92889.html</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_13</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz92888_pink_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>MOLLY SMITH MIX PRINT BANDEAU LACE TRIM MAXI DRESS</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/molly-smith-mix-print-bandeau-lace-trim-maxi-dress/GZZ92888.html</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_14</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz91922_red_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>MOLLY SMITH BANDEAU TWIST LACE MAXI DRESS</t>
+  </si>
+  <si>
+    <t>$31.50</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/molly-smith-bandeau-twist-lace-maxi-dress/GZZ91922.html</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_15</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/fzz45582_black_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>POLKA DOT SHIRT STYLE SKATER DRESS</t>
+  </si>
+  <si>
+    <t>$65.00</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/polka-dot-shirt-style-skater-dress/FZZ45582.html?color=105</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_16</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/bzz01304_light%20khaki_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>MATERNITY STRAPPY COWL NECK DRESS AND DUSTER COAT</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/maternity-strappy-cowl-neck-dress-and-duster-coat/BZZ01304.html</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_17</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz16285_black_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>PUFF SLEEVE RUCHED DETAIL MINI DRESS</t>
+  </si>
+  <si>
+    <t>$38.00</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/puff-sleeve-ruched-detail-mini-dress/GZZ16285.html?color=105</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_18</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz87436_black_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>PLUS NOUVELLE PRINTED T-SHIRT DRESS</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/plus-nouvelle-printed-t-shirt-dress/GZZ87436.html?color=105</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_19</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz81443_khaki_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>MATERNITY TEXTURED MIDI SMOCK DRESS</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/maternity-textured-midi-smock-dress/GZZ81443.html?color=135</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_20</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz42547_olive_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>PLUS RUFFLE STRAP MAXI DRESS</t>
+  </si>
+  <si>
+    <t>$40.00</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/plus-ruffle-strap-maxi-dress/GZZ42547.html?color=151</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_21</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz81102_hot%20pink_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>PLUS CHIFFON VOLUME SLEEVE MIDI SKATER DRESS</t>
+  </si>
+  <si>
+    <t>$50.00</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/plus-chiffon-volume-sleeve-midi-skater-dress/GZZ81102.html?color=535</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_22</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz18948_green_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>PLEATED SATIN OVERSIZED SLEEVE MIDI DRESS</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/pleated-satin-oversized-sleeve-midaxi-dress-/GZZ18948.html?color=105</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_23</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz04477_black_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>ONE SLEEVE DRAPE MINI DRESS</t>
+  </si>
+  <si>
+    <t>$25.00</t>
+  </si>
+  <si>
+    <t>https://ca.boohoo.com/one-sleeve-drape-mini-dress/GZZ04477.html?color=105</t>
+  </si>
+  <si>
+    <t>women_boohoo_dress_24</t>
+  </si>
+  <si>
+    <t>https://media.boohoo.com/i/boohoo/gzz81718_pink_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
+  </si>
+  <si>
+    <t>PLUS WOVEN ONE SHOULDER MINI DRESS</t>
   </si>
   <si>
     <t>$36.50</t>
   </si>
   <si>
-    <t>https://ca.boohoo.com/molly-smith-lace-trim-leopard-mesh-mini-dress/GZZ91938.html</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz91984_pink_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>MOLLY SMITH RUCHED SLINKY CUT OUT MAXI DRESS</t>
-  </si>
-  <si>
-    <t>$27.00</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/molly-smith-ruched-slinky-cut-out-maxi-dress/GZZ91984.html?color=155</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz94022_black_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>MOLLY SMITH SQUARE NECK STRAPPY LACE MAXI DRESS</t>
-  </si>
-  <si>
-    <t>$66.00</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/molly-smith-square-neck-strappy-lace-maxi-dress/GZZ94022.html?color=105</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz92887_brown_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>MOLLY SMITH MIX PRINT RUCHED MINI DRESS</t>
-  </si>
-  <si>
-    <t>$46.50</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/molly-smith-mix-print-ruched-mini-dress/GZZ92887.html</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz89419_white_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>MOLLY SMITH BANDEAU RUFFLE ASSYMETRIC DEVORE MINI DRESS</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/molly-smith-bandeau-ruffle-assymetric-devore-mini-dress/GZZ89419.html</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz92889_brown_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>MOLLY SMITH FLORAL TIE FRONT MAXI DRESS</t>
-  </si>
-  <si>
-    <t>$31.50</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/molly-smith-floral-tie-front-maxi-dress/GZZ92889.html</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz92888_pink_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>MOLLY SMITH MIX PRINT BANDEAU LACE TRIM MAXI DRESS</t>
-  </si>
-  <si>
-    <t>$63.00</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/molly-smith-mix-print-bandeau-lace-trim-maxi-dress/GZZ92888.html</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz91922_red_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>MOLLY SMITH BANDEAU TWIST LACE MAXI DRESS</t>
-  </si>
-  <si>
-    <t>$53.00</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/molly-smith-bandeau-twist-lace-maxi-dress/GZZ91922.html</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/bzz01304_light%20khaki_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>MATERNITY STRAPPY COWL NECK DRESS AND DUSTER COAT</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/maternity-strappy-cowl-neck-dress-and-duster-coat/BZZ01304.html</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/bzz01360_black_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>MATERNITY BASIC RIB BODYCON DRESS</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/maternity-basic-rib-bodycon-dress/BZZ01360.html?color=105</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz86162_black_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>PLUS PUFF SLEEVE SHIFT DRESS</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/plus-puff-sleeve-shift-dress-/GZZ86162.html?color=105</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz85024_tan_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>CRINKLE ROUCHED BARDOT MINI DRESS</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/crinkle-rouched-bardot-mini-dress/GZZ85024.html?color=166</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz11243_black_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>RIPPLE RIB LOW BACK BODYCON MIDI DRESS</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/ripple-rib-low-back-bodycon-midi-dress/GZZ11243.html?color=105</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz87430_stone_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>PLUS DSGN STUDIO PRINTED T-SHIRT DRESS</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/plus-dsgn-studio-printed-t-shirt-dress-/GZZ87430.html?color=165</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz89390_white_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>MATERNITY SHORT SLEEVE SPLIT HEM STRIPED DRESS</t>
-  </si>
-  <si>
-    <t>$50.00</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/maternity-short-sleeve-split-hem-striped-dress/GZZ89390.html?color=173</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz65301_red_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>BANDEAU RUFFLE MINI DRESS</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/bandeau-ruffle-mini-dress/GZZ65301.html?color=157</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz42547_olive_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>PLUS RUFFLE STRAP MAXI DRESS</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/plus-ruffle-strap-maxi-dress/GZZ42547.html?color=151</t>
-  </si>
-  <si>
-    <t>https://media.boohoo.com/i/boohoo/gzz04477_black_xl?w=900&amp;qlt=default&amp;fmt.jp2.qlt=70&amp;fmt=auto&amp;sm=fit</t>
-  </si>
-  <si>
-    <t>ONE SLEEVE DRAPE MINI DRESS</t>
-  </si>
-  <si>
-    <t>$26.50</t>
-  </si>
-  <si>
-    <t>https://ca.boohoo.com/one-sleeve-drape-mini-dress/GZZ04477.html?color=105</t>
+    <t>https://ca.boohoo.com/plus-woven-one-shoulder-mini-dress/GZZ81718.html?color=155</t>
   </si>
 </sst>
 </file>
@@ -383,462 +452,462 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s" s="0">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s" s="0">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="F14" t="s" s="0">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F15" t="s" s="0">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="F16" t="s" s="0">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C17" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="F17" t="s" s="0">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>6</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="F18" t="s" s="0">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F19" t="s" s="0">
-        <v>72</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F20" t="s" s="0">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D21" t="s" s="0">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="E21" t="s" s="0">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="F21" t="s" s="0">
-        <v>78</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="C22" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="E22" t="s" s="0">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="F22" t="s" s="0">
-        <v>82</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="C23" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="E23" t="s" s="0">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="F23" t="s" s="0">
-        <v>85</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="C24" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="E24" t="s" s="0">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>88</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>6</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="C25" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="E25" t="s" s="0">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="F25" t="s" s="0">
-        <v>92</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>